<commit_message>
Did some performance testing
</commit_message>
<xml_diff>
--- a/PerformanceEval.xlsx
+++ b/PerformanceEval.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s213898\Desktop\Git\ComplexGameSystems_ProceduralTerrain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AIE\GitHub\ComplexGameSystems_ProceduralTerrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF0446C-5EBD-4AF3-8C9F-7322554D2D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D51D15-3EA0-4C73-87AB-56B4DB62E3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,6 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2015,6 +2019,1941 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Map Data Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> by View Distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1316517577099528"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.78042527288295982"/>
+          <c:h val="0.57179024496937891"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Intel i7-9700K 8 Core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$42:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$44:$R$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4607038</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.47789310000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.48947679999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.47692430000000002</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.50259909999999997</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.50370130000000002</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.58978299999999995</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0.53471550000000001</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0.52372830000000004</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0.55488649999999995</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>0.54232409999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F129-45CC-AC30-17A15ABD552D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Intel i7-6700 4 Cores</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$8:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62919440000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65439800000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86757189999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70400110000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80734070000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.373472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1980329999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91477070000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1072059999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1792579999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4381060000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-F129-45CC-AC30-17A15ABD552D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="585353855"/>
+        <c:axId val="585350975"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="585353855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>View</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Distance</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585350975"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="585350975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585353855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18228430955482011"/>
+          <c:y val="0.88967519685039353"/>
+          <c:w val="0.6401235454016897"/>
+          <c:h val="0.10995479731700204"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Max</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Framerate by View Distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13271643722796067"/>
+          <c:y val="0.14856481481481484"/>
+          <c:w val="0.78474867847070828"/>
+          <c:h val="0.61808654126567508"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Intel i7-9700K 8 Core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2650160448739836E-2"/>
+                  <c:y val="-4.394685039370079E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-BADC-4DDE-97D9-F9F322A539A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$42:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$45:$R$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BADC-4DDE-97D9-F9F322A539A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Intel i7-6700 4 Core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$23:$R$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BADC-4DDE-97D9-F9F322A539A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="585350495"/>
+        <c:axId val="585353375"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="585350495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>View</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Distance</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585353375"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="585353375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585350495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19180071692936709"/>
+          <c:y val="0.89893445610965295"/>
+          <c:w val="0.62469794085310826"/>
+          <c:h val="0.10069553805774278"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Mesh</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Data Time by View Distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2507487734049883"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14364187759927655"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.77712567046708558"/>
+          <c:h val="0.59493839311752694"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Intel i7-9700K 8 Core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$57:$R$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$59:$R$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.3333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3998200000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.01038E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8175399999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.91882E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000000">
+                  <c:v>2.0610199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000000">
+                  <c:v>2.9209599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000000">
+                  <c:v>3.0562700000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000000">
+                  <c:v>3.05811E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000000">
+                  <c:v>3.8137799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000000">
+                  <c:v>3.5223699999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000000">
+                  <c:v>2.89419E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-179D-4191-9037-D03E3260187C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Intel i7-6700 4 Cores</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$22:$R$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.3333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26787480000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26583600000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20378309999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22714290000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32693729999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.257774</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.46378000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24118229999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26105499999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.202791</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23221800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-179D-4191-9037-D03E3260187C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="585348575"/>
+        <c:axId val="585349055"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="585348575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>View</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t> </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585349055"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="585349055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585348575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19156730639155059"/>
+          <c:y val="0.90819371536891225"/>
+          <c:w val="0.63994324382752699"/>
+          <c:h val="9.1436278798483497E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2175,6 +4114,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3724,6 +5783,1554 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4315,16 +7922,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>309161</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>7826</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80164</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4351,16 +7958,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>307829</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>78630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>6494</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>154830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4380,6 +7987,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>286978</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26BC13F9-8320-4A7E-2B5A-5ED1DFB311A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>3366</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>113718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>280789</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>189918</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95A0D1C-289F-D7BD-D4EC-358386F970E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>284612</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>187307</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>592135</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>73007</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B6C2E7-6388-7EF6-853D-6E448CC99EA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4653,11 +8368,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="J46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5278,7 +8996,7 @@
       <c r="B28">
         <v>45</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>0.46378000000000003</v>
       </c>
       <c r="D28">
@@ -5341,7 +9059,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -5349,12 +9067,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -5368,108 +9086,324 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>50</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
+      <c r="C42">
+        <v>0.04</v>
+      </c>
+      <c r="D42">
+        <v>178</v>
+      </c>
+      <c r="G42">
+        <v>50</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+      <c r="I42">
+        <v>150</v>
+      </c>
+      <c r="J42">
+        <v>200</v>
+      </c>
+      <c r="K42">
+        <v>250</v>
+      </c>
+      <c r="L42">
+        <v>300</v>
+      </c>
+      <c r="M42">
+        <v>350</v>
+      </c>
+      <c r="N42">
+        <v>400</v>
+      </c>
+      <c r="O42">
+        <v>450</v>
+      </c>
+      <c r="P42">
+        <v>500</v>
+      </c>
+      <c r="Q42">
+        <v>550</v>
+      </c>
+      <c r="R42">
+        <v>600</v>
+      </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>100</v>
       </c>
       <c r="B43">
         <v>9</v>
       </c>
+      <c r="C43" s="1">
+        <v>0.4607038</v>
+      </c>
+      <c r="D43">
+        <v>164</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>9</v>
+      </c>
+      <c r="I43">
+        <v>9</v>
+      </c>
+      <c r="J43">
+        <v>13</v>
+      </c>
+      <c r="K43">
+        <v>21</v>
+      </c>
+      <c r="L43">
+        <v>25</v>
+      </c>
+      <c r="M43">
+        <v>37</v>
+      </c>
+      <c r="N43">
+        <v>45</v>
+      </c>
+      <c r="O43">
+        <v>49</v>
+      </c>
+      <c r="P43">
+        <v>69</v>
+      </c>
+      <c r="Q43">
+        <v>69</v>
+      </c>
+      <c r="R43">
+        <v>89</v>
+      </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>150</v>
       </c>
       <c r="B44">
         <v>9</v>
       </c>
+      <c r="C44">
+        <v>0.47789310000000002</v>
+      </c>
+      <c r="D44">
+        <v>162</v>
+      </c>
+      <c r="G44">
+        <v>0.04</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.4607038</v>
+      </c>
+      <c r="I44">
+        <v>0.47789310000000002</v>
+      </c>
+      <c r="J44">
+        <v>0.48947679999999999</v>
+      </c>
+      <c r="K44">
+        <v>0.47692430000000002</v>
+      </c>
+      <c r="L44">
+        <v>0.50259909999999997</v>
+      </c>
+      <c r="M44">
+        <v>0.50370130000000002</v>
+      </c>
+      <c r="N44">
+        <v>0.58978299999999995</v>
+      </c>
+      <c r="O44">
+        <v>0.53471550000000001</v>
+      </c>
+      <c r="P44">
+        <v>0.52372830000000004</v>
+      </c>
+      <c r="Q44">
+        <v>0.55488649999999995</v>
+      </c>
+      <c r="R44">
+        <v>0.54232409999999998</v>
+      </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>200</v>
       </c>
       <c r="B45">
         <v>13</v>
       </c>
+      <c r="C45">
+        <v>0.48947679999999999</v>
+      </c>
+      <c r="D45">
+        <v>161</v>
+      </c>
+      <c r="G45">
+        <v>178</v>
+      </c>
+      <c r="H45">
+        <v>164</v>
+      </c>
+      <c r="I45">
+        <v>162</v>
+      </c>
+      <c r="J45">
+        <v>161</v>
+      </c>
+      <c r="K45">
+        <v>160</v>
+      </c>
+      <c r="L45">
+        <v>159</v>
+      </c>
+      <c r="M45">
+        <v>155</v>
+      </c>
+      <c r="N45">
+        <v>153</v>
+      </c>
+      <c r="O45">
+        <v>153</v>
+      </c>
+      <c r="P45">
+        <v>149</v>
+      </c>
+      <c r="Q45">
+        <v>146</v>
+      </c>
+      <c r="R45">
+        <v>142</v>
+      </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>250</v>
       </c>
       <c r="B46">
         <v>21</v>
       </c>
+      <c r="C46">
+        <v>0.47692430000000002</v>
+      </c>
+      <c r="D46">
+        <v>160</v>
+      </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>300</v>
       </c>
       <c r="B47">
         <v>25</v>
       </c>
+      <c r="C47">
+        <v>0.50259909999999997</v>
+      </c>
+      <c r="D47">
+        <v>159</v>
+      </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>350</v>
       </c>
       <c r="B48">
         <v>37</v>
       </c>
+      <c r="C48">
+        <v>0.50370130000000002</v>
+      </c>
+      <c r="D48">
+        <v>155</v>
+      </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>400</v>
       </c>
       <c r="B49">
         <v>45</v>
       </c>
+      <c r="C49">
+        <v>0.58978299999999995</v>
+      </c>
+      <c r="D49">
+        <v>153</v>
+      </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>450</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
+      <c r="C50">
+        <v>0.53471550000000001</v>
+      </c>
+      <c r="D50">
+        <v>153</v>
+      </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>500</v>
       </c>
       <c r="B51">
         <v>69</v>
       </c>
+      <c r="C51">
+        <v>0.52372830000000004</v>
+      </c>
+      <c r="D51">
+        <v>149</v>
+      </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>550</v>
       </c>
       <c r="B52">
         <v>69</v>
       </c>
+      <c r="C52">
+        <v>0.55488649999999995</v>
+      </c>
+      <c r="D52">
+        <v>146</v>
+      </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>600</v>
       </c>
       <c r="B53">
         <v>89</v>
       </c>
+      <c r="C53">
+        <v>0.54232409999999998</v>
+      </c>
+      <c r="D53">
+        <v>142</v>
+      </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -5483,104 +9417,322 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>50</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
+      <c r="C57">
+        <v>0.3333333</v>
+      </c>
+      <c r="D57">
+        <v>178</v>
+      </c>
+      <c r="G57">
+        <v>50</v>
+      </c>
+      <c r="H57">
+        <v>100</v>
+      </c>
+      <c r="I57">
+        <v>150</v>
+      </c>
+      <c r="J57">
+        <v>200</v>
+      </c>
+      <c r="K57">
+        <v>250</v>
+      </c>
+      <c r="L57">
+        <v>300</v>
+      </c>
+      <c r="M57">
+        <v>350</v>
+      </c>
+      <c r="N57">
+        <v>400</v>
+      </c>
+      <c r="O57">
+        <v>450</v>
+      </c>
+      <c r="P57">
+        <v>500</v>
+      </c>
+      <c r="Q57">
+        <v>550</v>
+      </c>
+      <c r="R57">
+        <v>600</v>
+      </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>100</v>
       </c>
       <c r="B58">
         <v>9</v>
       </c>
+      <c r="C58">
+        <v>5.3998200000000003E-2</v>
+      </c>
+      <c r="D58">
+        <v>164</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>9</v>
+      </c>
+      <c r="I58">
+        <v>9</v>
+      </c>
+      <c r="J58">
+        <v>13</v>
+      </c>
+      <c r="K58">
+        <v>21</v>
+      </c>
+      <c r="L58">
+        <v>25</v>
+      </c>
+      <c r="M58">
+        <v>37</v>
+      </c>
+      <c r="N58">
+        <v>45</v>
+      </c>
+      <c r="O58">
+        <v>49</v>
+      </c>
+      <c r="P58">
+        <v>69</v>
+      </c>
+      <c r="Q58">
+        <v>69</v>
+      </c>
+      <c r="R58">
+        <v>89</v>
+      </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>150</v>
       </c>
       <c r="B59">
         <v>9</v>
       </c>
+      <c r="C59">
+        <v>3.01038E-2</v>
+      </c>
+      <c r="D59">
+        <v>162</v>
+      </c>
+      <c r="G59">
+        <v>0.3333333</v>
+      </c>
+      <c r="H59">
+        <v>5.3998200000000003E-2</v>
+      </c>
+      <c r="I59">
+        <v>3.01038E-2</v>
+      </c>
+      <c r="J59">
+        <v>6.8175399999999997E-2</v>
+      </c>
+      <c r="K59">
+        <v>7.91882E-2</v>
+      </c>
+      <c r="L59" s="1">
+        <v>2.0610199999999999E-2</v>
+      </c>
+      <c r="M59" s="1">
+        <v>2.9209599999999999E-2</v>
+      </c>
+      <c r="N59" s="1">
+        <v>3.0562700000000002E-2</v>
+      </c>
+      <c r="O59" s="1">
+        <v>3.05811E-2</v>
+      </c>
+      <c r="P59" s="1">
+        <v>3.8137799999999999E-2</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>3.5223699999999997E-2</v>
+      </c>
+      <c r="R59" s="1">
+        <v>2.89419E-2</v>
+      </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>200</v>
       </c>
       <c r="B60">
         <v>13</v>
       </c>
+      <c r="C60">
+        <v>6.8175399999999997E-2</v>
+      </c>
+      <c r="D60">
+        <v>161</v>
+      </c>
+      <c r="G60">
+        <v>178</v>
+      </c>
+      <c r="H60">
+        <v>164</v>
+      </c>
+      <c r="I60">
+        <v>162</v>
+      </c>
+      <c r="J60">
+        <v>161</v>
+      </c>
+      <c r="K60">
+        <v>160</v>
+      </c>
+      <c r="L60">
+        <v>159</v>
+      </c>
+      <c r="M60">
+        <v>155</v>
+      </c>
+      <c r="N60">
+        <v>153</v>
+      </c>
+      <c r="O60">
+        <v>153</v>
+      </c>
+      <c r="P60">
+        <v>149</v>
+      </c>
+      <c r="Q60">
+        <v>146</v>
+      </c>
+      <c r="R60">
+        <v>142</v>
+      </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>250</v>
       </c>
       <c r="B61">
         <v>21</v>
       </c>
+      <c r="C61">
+        <v>7.91882E-2</v>
+      </c>
+      <c r="D61">
+        <v>160</v>
+      </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>300</v>
       </c>
       <c r="B62">
         <v>25</v>
       </c>
+      <c r="C62" s="1">
+        <v>2.0610199999999999E-2</v>
+      </c>
+      <c r="D62">
+        <v>159</v>
+      </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>350</v>
       </c>
       <c r="B63">
         <v>37</v>
       </c>
+      <c r="C63" s="1">
+        <v>2.9209599999999999E-2</v>
+      </c>
+      <c r="D63">
+        <v>155</v>
+      </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>400</v>
       </c>
       <c r="B64">
         <v>45</v>
       </c>
+      <c r="C64" s="1">
+        <v>3.0562700000000002E-2</v>
+      </c>
+      <c r="D64">
+        <v>153</v>
+      </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>450</v>
       </c>
       <c r="B65">
         <v>49</v>
       </c>
+      <c r="C65" s="1">
+        <v>3.05811E-2</v>
+      </c>
+      <c r="D65">
+        <v>153</v>
+      </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>500</v>
       </c>
       <c r="B66">
         <v>69</v>
       </c>
+      <c r="C66" s="1">
+        <v>3.8137799999999999E-2</v>
+      </c>
+      <c r="D66">
+        <v>149</v>
+      </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>550</v>
       </c>
       <c r="B67">
         <v>69</v>
       </c>
+      <c r="C67" s="1">
+        <v>3.5223699999999997E-2</v>
+      </c>
+      <c r="D67">
+        <v>146</v>
+      </c>
+      <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>600</v>
       </c>
       <c r="B68">
         <v>89</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2.89419E-2</v>
+      </c>
+      <c r="D68">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>